<commit_message>
Update NS Diagram- Assignment1.xlsx
</commit_message>
<xml_diff>
--- a/NS Diagram- Assignment1.xlsx
+++ b/NS Diagram- Assignment1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://heriotwatt-my.sharepoint.com/personal/ch72_hw_ac_uk/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conno\Documents\GitHub\EmbeddedSoftware-Assignment1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EBFAE881-BF28-4BA9-B8B1-6F3B8084CCC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FCFD510C-229F-4796-A8B0-2A31B2732C4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="19543" windowHeight="13097" xr2:uid="{6C8379BB-D26F-4DFF-BC64-52811643F3CB}"/>
   </bookViews>
@@ -969,14 +969,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>195964</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>185056</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>195963</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>2</xdr:rowOff>
     </xdr:to>
@@ -993,7 +993,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="805544" y="2220685"/>
+          <a:off x="3015364" y="2220685"/>
           <a:ext cx="2215242" cy="370117"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1036,14 +1036,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>195964</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>195963</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>2</xdr:rowOff>
     </xdr:to>
@@ -1060,7 +1060,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="805544" y="2590801"/>
+          <a:off x="3015364" y="2590801"/>
           <a:ext cx="2215242" cy="370115"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1103,14 +1103,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>195963</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>2</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>201385</xdr:colOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>195962</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>2</xdr:rowOff>
     </xdr:to>
@@ -1127,7 +1127,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="805543" y="2960916"/>
+          <a:off x="3015363" y="2960916"/>
           <a:ext cx="2215242" cy="370115"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1170,14 +1170,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>195963</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>2</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>201385</xdr:colOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>195962</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -1194,7 +1194,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="805543" y="3331031"/>
+          <a:off x="3015363" y="3331031"/>
           <a:ext cx="2215242" cy="1480455"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1732,14 +1732,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>195963</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>185056</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>195963</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -1756,7 +1756,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1006929" y="3701142"/>
+          <a:off x="3216749" y="3701142"/>
           <a:ext cx="2013857" cy="370115"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1803,14 +1803,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>195963</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>195963</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:to>
@@ -1827,7 +1827,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1006929" y="4071257"/>
+          <a:off x="3216749" y="4071257"/>
           <a:ext cx="2013857" cy="370115"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1874,14 +1874,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>195963</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>195963</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -1898,7 +1898,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1006929" y="4441371"/>
+          <a:off x="3216749" y="4441371"/>
           <a:ext cx="2013857" cy="370115"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2242,7 +2242,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="AG11" sqref="AG11"/>
+      <selection activeCell="AD24" sqref="AD24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2253,6 +2253,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007631A97BB086F84CB8DE9F7E73C7BA4D" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d83f6cfe591fed3af8c2af13687732e8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="ffbeba94-ea97-4897-bb8b-36df93c0497c" xmlns:ns4="47675ea1-c95d-4668-843b-97cbcc99f11f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0dfce47bf986ec4318c1d7ebbd1e1f7f" ns3:_="" ns4:_="">
     <xsd:import namespace="ffbeba94-ea97-4897-bb8b-36df93c0497c"/>
@@ -2463,22 +2478,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95853F0C-9DAB-44F1-B887-B06C57288C16}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="47675ea1-c95d-4668-843b-97cbcc99f11f"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="ffbeba94-ea97-4897-bb8b-36df93c0497c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{30EB9417-57E1-41C5-B764-9DAC1B6E0015}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{736FBCE1-8BAD-495F-97D7-9F762C3A88E7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2495,29 +2520,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{30EB9417-57E1-41C5-B764-9DAC1B6E0015}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95853F0C-9DAB-44F1-B887-B06C57288C16}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="47675ea1-c95d-4668-843b-97cbcc99f11f"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="ffbeba94-ea97-4897-bb8b-36df93c0497c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>